<commit_message>
Changes done on main
</commit_message>
<xml_diff>
--- a/StockReport/Stock_Report_2026-01-14_Final.xlsx
+++ b/StockReport/Stock_Report_2026-01-14_Final.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -614,7 +614,7 @@
         <v>476341.253968254</v>
       </c>
       <c r="N3" t="n">
-        <v>2124</v>
+        <v>2059.15</v>
       </c>
       <c r="O3" t="n">
         <v>1451.95</v>
@@ -1824,7 +1824,7 @@
         <v>359124.3015873016</v>
       </c>
       <c r="N25" t="n">
-        <v>571.5</v>
+        <v>556</v>
       </c>
       <c r="O25" t="n">
         <v>217.95</v>
@@ -2704,8 +2704,12 @@
       <c r="C42" t="n">
         <v>185.05</v>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>910.05</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-0.796659524201967</v>
+      </c>
       <c r="F42" t="n">
         <v>-0.8196569535133028</v>
       </c>

</xml_diff>